<commit_message>
updated BASoBC, TCCpUCD, CSpULApYbp
</commit_message>
<xml_diff>
--- a/InputData/elec/TCCpUCD/Trans Const Cost per Unit Cap Dist.xlsx
+++ b/InputData/elec/TCCpUCD/Trans Const Cost per Unit Cap Dist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26306"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26307"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pembinainstitute.sharepoint.com/sites/PRO-EnergyPolicySimulator2021/Shared Documents/Research and Analysis/eps-canada-1.4.3/InputData/elec/TCCpUCD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="11_E7049D8AAF947B6FB8817C9DACB0FB7CD6E92B9C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62953F3E-3967-4FF6-A68D-41662842250B}"/>
+  <xr:revisionPtr revIDLastSave="151" documentId="11_E7049D8AAF947B6FB8817C9DACB0FB7CD6E92B9C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7D168E8-E77E-41F7-B661-DED3FFF5C7C3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>TCCpUCD Transmission Construction Cost per Unit Capacity Distance</t>
   </si>
@@ -61,6 +61,21 @@
     <t>Value is a 5-year average from 2017-2021</t>
   </si>
   <si>
+    <t xml:space="preserve">Source: </t>
+  </si>
+  <si>
+    <t>Alberta Chambers of Commerce</t>
+  </si>
+  <si>
+    <t>2022 Report</t>
+  </si>
+  <si>
+    <t>MW-Miles example to use in calculations</t>
+  </si>
+  <si>
+    <t>https://www.abchamber.ca/wp-content/uploads/2022/02/Strengthening-Albertas-Electricity-Transmission-Intertie-Infrastructure.pdf</t>
+  </si>
+  <si>
     <t>Item</t>
   </si>
   <si>
@@ -124,7 +139,41 @@
     <t>Total (2012$USD/mile)</t>
   </si>
   <si>
-    <t>Cost per Distance (USD$2012/mile)</t>
+    <t>Transmission line length (miles)</t>
+  </si>
+  <si>
+    <t>Transmission line voltage (kv)</t>
+  </si>
+  <si>
+    <t>Transmission line capacity (MW)</t>
+  </si>
+  <si>
+    <t>Transmission line MW-miles</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Note</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>: See Alberta Chambers of Commerce data source for values - Montana Alberta Transmission Line specs used as example</t>
+    </r>
+  </si>
+  <si>
+    <t>Cost (2012 $USD/MW-Mile)</t>
+  </si>
+  <si>
+    <t>Cost per capacity distance (USD$2012/MW-mile)</t>
   </si>
   <si>
     <t>Transmission Construction</t>
@@ -134,7 +183,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,8 +233,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -192,6 +255,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -261,7 +330,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -271,6 +340,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Body: normal cell" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -616,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -670,9 +741,33 @@
         <v>7</v>
       </c>
     </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="B16" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" xr:uid="{57B399CA-529B-41AA-B301-B002FF8CF722}"/>
+    <hyperlink ref="B16" r:id="rId2" xr:uid="{911465E3-39C4-4BBE-997F-7ED26303E749}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -680,10 +775,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -695,15 +790,15 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>110349</v>
@@ -712,7 +807,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>17274</v>
@@ -720,7 +815,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>11449</v>
@@ -728,7 +823,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>67722</v>
@@ -736,7 +831,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B6">
         <v>600195</v>
@@ -744,7 +839,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B7">
         <v>52757</v>
@@ -752,7 +847,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B8">
         <v>30646</v>
@@ -760,7 +855,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B9">
         <v>15985</v>
@@ -768,7 +863,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B10">
         <v>112018</v>
@@ -776,7 +871,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B11">
         <v>10205</v>
@@ -784,7 +879,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B12">
         <v>143769</v>
@@ -792,7 +887,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B13">
         <v>15128</v>
@@ -800,7 +895,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B14">
         <v>145790</v>
@@ -808,7 +903,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B15">
         <v>19563</v>
@@ -816,48 +911,97 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B16" s="6">
         <f>SUM(B2:B15)</f>
         <v>1352850</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:5">
       <c r="A18" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B18">
         <v>0.62137100000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:5">
       <c r="B19" s="3"/>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B20">
         <f>B16*B18</f>
         <v>840621.75734999997</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B22">
         <v>0.72229090790676931</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B24">
         <f>B20*B22</f>
         <v>607173.45232251543</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26">
+        <f>344*B18</f>
+        <v>213.75162399999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27">
+        <v>240</v>
+      </c>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29">
+        <f>B26*B28</f>
+        <v>64125.487199999996</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="7">
+        <f>(B24*B26)/B29</f>
+        <v>2023.911507741718</v>
       </c>
     </row>
   </sheetData>
@@ -872,8 +1016,8 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -884,16 +1028,16 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B2" s="5">
-        <f>Data!B24</f>
-        <v>607173.45232251543</v>
+        <f>Data!B32</f>
+        <v>2023.911507741718</v>
       </c>
     </row>
   </sheetData>
@@ -902,6 +1046,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <of2ed5e60f3c4f8984f283882cb94320 xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </of2ed5e60f3c4f8984f283882cb94320>
+    <ff7c4ad8664a4671b57370e258acad6a xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ff7c4ad8664a4671b57370e258acad6a>
+    <l787e5950a9249679d0130235a9a791b xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l787e5950a9249679d0130235a9a791b>
+    <TaxCatchAll xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="de340059-046a-4f1a-8b62-ade039df3700">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010010EB76B7FE121F489C7B2A4727FCE3E9" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fdee17017a9ad5b872047a216f95da93">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="52604411-7aeb-406e-8b34-4ce79a7293cc" xmlns:ns3="de340059-046a-4f1a-8b62-ade039df3700" xmlns:ns4="d580559a-617d-4d7d-8fb9-71ff64b58360" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="37825e9edfcb807d863c63152c6d8635" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="52604411-7aeb-406e-8b34-4ce79a7293cc"/>
@@ -1161,43 +1334,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <of2ed5e60f3c4f8984f283882cb94320 xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </of2ed5e60f3c4f8984f283882cb94320>
-    <ff7c4ad8664a4671b57370e258acad6a xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ff7c4ad8664a4671b57370e258acad6a>
-    <l787e5950a9249679d0130235a9a791b xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l787e5950a9249679d0130235a9a791b>
-    <TaxCatchAll xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="de340059-046a-4f1a-8b62-ade039df3700">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2ED55DB-2ADA-4181-A08B-E08D10A805C1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A76B0ABF-00FF-4637-8665-A787BE55DA4F}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A76B0ABF-00FF-4637-8665-A787BE55DA4F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C9CE083-6688-4054-93F1-7E15F57A69BD}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C9CE083-6688-4054-93F1-7E15F57A69BD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2ED55DB-2ADA-4181-A08B-E08D10A805C1}"/>
 </file>
</xml_diff>